<commit_message>
added in back testing script to test other models out at scale
</commit_message>
<xml_diff>
--- a/RF Lifetime Predictions.xlsx
+++ b/RF Lifetime Predictions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thigg\Desktop\Hockey Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9CFA298-BFBA-47D8-AE56-5EA7BDE77B41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177CA95C-CBCB-4690-95AE-5742F83060F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId3"/>
+    <pivotCache cacheId="13" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -516,7 +516,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -714,6 +714,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -876,7 +882,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -893,6 +899,7 @@
     <xf numFmtId="164" fontId="0" fillId="34" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="35" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
@@ -954,7 +961,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Thomas Higgins" refreshedDate="45311.547893055555" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="311" xr:uid="{DA5DA62F-86DF-48F4-B83B-306BE2A00D1E}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Thomas Higgins" refreshedDate="45311.758368981478" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="311" xr:uid="{DA5DA62F-86DF-48F4-B83B-306BE2A00D1E}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:O1048576" sheet="Predictions"/>
   </cacheSource>
@@ -6412,7 +6419,7 @@
     <s v="Arizona Coyotes"/>
     <n v="0.42399999999999999"/>
     <s v="Playing At:  Arizona Coyotes   Home"/>
-    <n v="1"/>
+    <n v="0"/>
     <x v="4"/>
     <m/>
     <m/>
@@ -6510,7 +6517,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FF87AC2C-F765-45B0-A26D-AAA33F3641F7}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FF87AC2C-F765-45B0-A26D-AAA33F3641F7}" name="PivotTable1" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A5:C11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="16">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
@@ -6801,7 +6808,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{356A29A8-7537-4F34-9050-3E279C8F33A9}" name="PivotTable3" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{356A29A8-7537-4F34-9050-3E279C8F33A9}" name="PivotTable3" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="L3:N12" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField axis="axisRow" showAll="0">
@@ -7193,7 +7200,7 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7249,10 +7256,10 @@
       <c r="L4" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="M4" s="14">
+      <c r="M4" s="15">
         <v>24</v>
       </c>
-      <c r="N4" s="14">
+      <c r="N4" s="15">
         <v>18</v>
       </c>
       <c r="O4" s="5">
@@ -7285,10 +7292,10 @@
       <c r="L5" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="M5" s="14">
+      <c r="M5" s="15">
         <v>42</v>
       </c>
-      <c r="N5" s="14">
+      <c r="N5" s="15">
         <v>24</v>
       </c>
       <c r="O5" s="5">
@@ -7300,10 +7307,10 @@
       <c r="A6" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B6" s="14">
+      <c r="B6" s="15">
         <v>6</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="15">
         <v>5</v>
       </c>
       <c r="D6" s="6">
@@ -7325,10 +7332,10 @@
       <c r="L6" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="M6" s="14">
+      <c r="M6" s="15">
         <v>10</v>
       </c>
-      <c r="N6" s="14">
+      <c r="N6" s="15">
         <v>5</v>
       </c>
       <c r="O6" s="5">
@@ -7340,10 +7347,10 @@
       <c r="A7" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="15">
         <v>15</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="15">
         <v>11</v>
       </c>
       <c r="D7" s="6">
@@ -7352,7 +7359,7 @@
       </c>
       <c r="E7" s="10">
         <f>SUM(C9:C10)</f>
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F7" s="8">
         <f>SUM(C6:C8)</f>
@@ -7365,10 +7372,10 @@
       <c r="L7" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="M7" s="14">
+      <c r="M7" s="15">
         <v>30</v>
       </c>
-      <c r="N7" s="14">
+      <c r="N7" s="15">
         <v>16</v>
       </c>
       <c r="O7" s="5">
@@ -7380,10 +7387,10 @@
       <c r="A8" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B8" s="14">
+      <c r="B8" s="15">
         <v>65</v>
       </c>
-      <c r="C8" s="14">
+      <c r="C8" s="15">
         <v>42</v>
       </c>
       <c r="D8" s="6">
@@ -7392,7 +7399,7 @@
       </c>
       <c r="E8" s="11">
         <f>E7/E6</f>
-        <v>0.5580357142857143</v>
+        <v>0.5535714285714286</v>
       </c>
       <c r="F8" s="9">
         <f>F7/F6</f>
@@ -7405,10 +7412,10 @@
       <c r="L8" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="M8" s="14">
+      <c r="M8" s="15">
         <v>50</v>
       </c>
-      <c r="N8" s="14">
+      <c r="N8" s="15">
         <v>31</v>
       </c>
       <c r="O8" s="5">
@@ -7420,10 +7427,10 @@
       <c r="A9" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="15">
         <v>124</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="15">
         <v>73</v>
       </c>
       <c r="D9" s="6">
@@ -7433,10 +7440,10 @@
       <c r="L9" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="M9" s="14">
+      <c r="M9" s="15">
         <v>61</v>
       </c>
-      <c r="N9" s="14">
+      <c r="N9" s="15">
         <v>34</v>
       </c>
       <c r="O9" s="5">
@@ -7448,23 +7455,23 @@
       <c r="A10" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B10" s="14">
+      <c r="B10" s="15">
         <v>100</v>
       </c>
-      <c r="C10" s="14">
-        <v>52</v>
+      <c r="C10" s="15">
+        <v>51</v>
       </c>
       <c r="D10" s="6">
         <f t="shared" si="1"/>
-        <v>0.52</v>
+        <v>0.51</v>
       </c>
       <c r="L10" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="M10" s="14">
+      <c r="M10" s="15">
         <v>44</v>
       </c>
-      <c r="N10" s="14">
+      <c r="N10" s="15">
         <v>27</v>
       </c>
       <c r="O10" s="5">
@@ -7476,39 +7483,39 @@
       <c r="A11" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B11" s="14">
+      <c r="B11" s="15">
         <v>310</v>
       </c>
-      <c r="C11" s="14">
-        <v>183</v>
+      <c r="C11" s="15">
+        <v>182</v>
       </c>
       <c r="D11" s="6">
         <f t="shared" si="1"/>
-        <v>0.5903225806451613</v>
+        <v>0.58709677419354833</v>
       </c>
       <c r="L11" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="M11" s="14">
+      <c r="M11" s="15">
         <v>49</v>
       </c>
-      <c r="N11" s="14">
-        <v>28</v>
+      <c r="N11" s="15">
+        <v>27</v>
       </c>
       <c r="O11" s="5">
         <f t="shared" si="0"/>
-        <v>0.5714285714285714</v>
+        <v>0.55102040816326525</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="L12" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="M12" s="14">
+      <c r="M12" s="15">
         <v>310</v>
       </c>
-      <c r="N12" s="14">
-        <v>183</v>
+      <c r="N12" s="15">
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -7521,8 +7528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O311"/>
   <sheetViews>
-    <sheetView topLeftCell="A279" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H300" sqref="H300:H311"/>
+    <sheetView topLeftCell="A276" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H311" sqref="H311"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17934,7 +17941,7 @@
       <c r="G304" t="s">
         <v>69</v>
       </c>
-      <c r="H304">
+      <c r="H304" s="14">
         <v>1</v>
       </c>
       <c r="I304" t="str" cm="1">
@@ -17994,7 +18001,7 @@
       <c r="G306" t="s">
         <v>78</v>
       </c>
-      <c r="H306">
+      <c r="H306" s="14">
         <v>1</v>
       </c>
       <c r="I306" t="str" cm="1">
@@ -18024,8 +18031,8 @@
       <c r="G307" t="s">
         <v>80</v>
       </c>
-      <c r="H307">
-        <v>1</v>
+      <c r="H307" s="14">
+        <v>0</v>
       </c>
       <c r="I307" t="str" cm="1">
         <f t="array" ref="I307">_xlfn.IFS(D307 &gt;= 0.85, "85 &lt;", AND(D307 &gt;=0.8, D307 &lt; 0.85), "80-85", AND(D307 &gt;= 0.7, D307 &lt; 0.8), "70-80", AND(D307 &gt;= 0.6, D307 &lt; 0.7),  "60-70", AND(D307 &gt;= 0.5, D307 &lt; 0.6), "50-60")</f>
@@ -18144,7 +18151,7 @@
       <c r="G311" t="s">
         <v>49</v>
       </c>
-      <c r="H311">
+      <c r="H311" s="14">
         <v>0</v>
       </c>
       <c r="I311" t="str" cm="1">

</xml_diff>

<commit_message>
added in pda modeling, will continue to monitor pda version
</commit_message>
<xml_diff>
--- a/RF Lifetime Predictions.xlsx
+++ b/RF Lifetime Predictions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thigg\Desktop\Hockey Models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177CA95C-CBCB-4690-95AE-5742F83060F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DD0CCD1-0007-4F21-B17F-B7CCCD03E824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="13" r:id="rId3"/>
+    <pivotCache cacheId="16" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -961,7 +961,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Thomas Higgins" refreshedDate="45311.758368981478" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="311" xr:uid="{DA5DA62F-86DF-48F4-B83B-306BE2A00D1E}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Thomas Higgins" refreshedDate="45311.879465162034" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="311" xr:uid="{DA5DA62F-86DF-48F4-B83B-306BE2A00D1E}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:O1048576" sheet="Predictions"/>
   </cacheSource>
@@ -6334,7 +6334,7 @@
     <s v="Toronto Maple Leafs"/>
     <n v="0.34799999999999998"/>
     <s v="Playing At:  Vancouver Canucks   Home"/>
-    <n v="0"/>
+    <n v="1"/>
     <x v="3"/>
     <m/>
     <m/>
@@ -6517,7 +6517,100 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FF87AC2C-F765-45B0-A26D-AAA33F3641F7}" name="PivotTable1" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{356A29A8-7537-4F34-9050-3E279C8F33A9}" name="PivotTable3" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="L3:N12" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="16">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="10">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item h="1" x="8"/>
+        <item x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField numFmtId="14" showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="2">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+  </colItems>
+  <dataFields count="2">
+    <dataField name="Count of Winner" fld="2" subtotal="count" baseField="0" baseItem="0"/>
+    <dataField name="Sum of Model" fld="7" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{FF87AC2C-F765-45B0-A26D-AAA33F3641F7}" name="PivotTable1" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A5:C11" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="3" colPageCount="1"/>
   <pivotFields count="16">
     <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
@@ -6791,99 +6884,6 @@
     <pageField fld="1" hier="-1"/>
     <pageField fld="3" hier="-1"/>
   </pageFields>
-  <dataFields count="2">
-    <dataField name="Count of Winner" fld="2" subtotal="count" baseField="0" baseItem="0"/>
-    <dataField name="Sum of Model" fld="7" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{356A29A8-7537-4F34-9050-3E279C8F33A9}" name="PivotTable3" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="L3:N12" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="16">
-    <pivotField axis="axisRow" showAll="0">
-      <items count="10">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item h="1" x="8"/>
-        <item x="7"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField numFmtId="14" showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="0"/>
-  </rowFields>
-  <rowItems count="9">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="2">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-  </colItems>
   <dataFields count="2">
     <dataField name="Count of Winner" fld="2" subtotal="count" baseField="0" baseItem="0"/>
     <dataField name="Sum of Model" fld="7" baseField="0" baseItem="0"/>
@@ -7200,7 +7200,7 @@
   <dimension ref="A1:O12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7359,7 +7359,7 @@
       </c>
       <c r="E7" s="10">
         <f>SUM(C9:C10)</f>
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F7" s="8">
         <f>SUM(C6:C8)</f>
@@ -7399,7 +7399,7 @@
       </c>
       <c r="E8" s="11">
         <f>E7/E6</f>
-        <v>0.5535714285714286</v>
+        <v>0.5580357142857143</v>
       </c>
       <c r="F8" s="9">
         <f>F7/F6</f>
@@ -7431,11 +7431,11 @@
         <v>124</v>
       </c>
       <c r="C9" s="15">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D9" s="6">
         <f t="shared" si="1"/>
-        <v>0.58870967741935487</v>
+        <v>0.59677419354838712</v>
       </c>
       <c r="L9" s="4" t="s">
         <v>98</v>
@@ -7487,11 +7487,11 @@
         <v>310</v>
       </c>
       <c r="C11" s="15">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="D11" s="6">
         <f t="shared" si="1"/>
-        <v>0.58709677419354833</v>
+        <v>0.5903225806451613</v>
       </c>
       <c r="L11" s="4" t="s">
         <v>100</v>
@@ -7500,11 +7500,11 @@
         <v>49</v>
       </c>
       <c r="N11" s="15">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="O11" s="5">
         <f t="shared" si="0"/>
-        <v>0.55102040816326525</v>
+        <v>0.5714285714285714</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
@@ -7515,7 +7515,7 @@
         <v>310</v>
       </c>
       <c r="N12" s="15">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -7528,8 +7528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O311"/>
   <sheetViews>
-    <sheetView topLeftCell="A276" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H311" sqref="H311"/>
+    <sheetView topLeftCell="A267" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H310" sqref="H310"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17882,7 +17882,7 @@
         <v>46</v>
       </c>
       <c r="H302">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I302" t="str" cm="1">
         <f t="array" ref="I302">_xlfn.IFS(D302 &gt;= 0.85, "85 &lt;", AND(D302 &gt;=0.8, D302 &lt; 0.85), "80-85", AND(D302 &gt;= 0.7, D302 &lt; 0.8), "70-80", AND(D302 &gt;= 0.6, D302 &lt; 0.7),  "60-70", AND(D302 &gt;= 0.5, D302 &lt; 0.6), "50-60")</f>

</xml_diff>